<commit_message>
using role name ot unit code to assign users to roles
</commit_message>
<xml_diff>
--- a/Role users  v1.1.xlsx
+++ b/Role users  v1.1.xlsx
@@ -28,33 +28,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>user3</t>
   </si>
   <si>
-    <t>aa</t>
+    <t>mfa_remon</t>
+  </si>
+  <si>
+    <t>mfa_omar</t>
+  </si>
+  <si>
+    <t>youssef1</t>
+  </si>
+  <si>
+    <t>mf1</t>
+  </si>
+  <si>
+    <t>mfa_salam</t>
   </si>
   <si>
     <t>مدير اجازه دراسيه بمرتب</t>
-  </si>
-  <si>
-    <t>اعاره من الوزاره</t>
-  </si>
-  <si>
-    <t>mfa_remon</t>
-  </si>
-  <si>
-    <t>mfa_omar</t>
-  </si>
-  <si>
-    <t>youssef1</t>
-  </si>
-  <si>
-    <t>mf1</t>
-  </si>
-  <si>
-    <t>mfa_salam</t>
   </si>
 </sst>
 </file>
@@ -378,7 +372,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,23 +384,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -414,29 +408,30 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>